<commit_message>
Inserita nuova versione di BlocksScanner - implementata distinzione contratti verificati e non.
</commit_message>
<xml_diff>
--- a/Grafici/Grafico 2 - OpcodeContrattiVerificati.xlsx
+++ b/Grafici/Grafico 2 - OpcodeContrattiVerificati.xlsx
@@ -1359,12 +1359,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="172194816"/>
-        <c:axId val="162318592"/>
+        <c:axId val="177838080"/>
+        <c:axId val="167930112"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="172194816"/>
+        <c:axId val="177838080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1373,7 +1373,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="162318592"/>
+        <c:crossAx val="167930112"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1381,7 +1381,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="162318592"/>
+        <c:axId val="167930112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1392,7 +1392,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="172194816"/>
+        <c:crossAx val="177838080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1414,15 +1414,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>257174</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>180974</xdr:rowOff>
+      <xdr:colOff>9523</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>19049</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>28</xdr:col>
-      <xdr:colOff>381000</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>600074</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1733,8 +1733,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:B136"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A53" sqref="A53:XFD53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>